<commit_message>
update data and figures
</commit_message>
<xml_diff>
--- a/dados/ZEE_AP_basedados_sig.xlsx
+++ b/dados/ZEE_AP_basedados_sig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="420" windowWidth="17955" windowHeight="5685" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="420" windowWidth="17955" windowHeight="5685"/>
   </bookViews>
   <sheets>
     <sheet name="metadados" sheetId="2" r:id="rId1"/>
@@ -3367,9 +3367,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K257"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="14" topLeftCell="A255" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H258" sqref="H258"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8449,7 +8449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IJ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="11" ySplit="1" topLeftCell="IG29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>